<commit_message>
simplifikasi decition on v1 v2 v3
</commit_message>
<xml_diff>
--- a/Data/Pengujian/closelist_512_Avg10_AllComb.xlsx
+++ b/Data/Pengujian/closelist_512_Avg10_AllComb.xlsx
@@ -714,257 +714,257 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BD</t>
+          <t>BDS</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>454</v>
+        <v>369</v>
       </c>
       <c r="C18" t="n">
-        <v>1793</v>
+        <v>1419</v>
       </c>
       <c r="D18" t="n">
-        <v>7136</v>
+        <v>5434</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BD-PPO</t>
+          <t>BDS-PPO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>454</v>
+        <v>369</v>
       </c>
       <c r="C19" t="n">
-        <v>1793</v>
+        <v>1419</v>
       </c>
       <c r="D19" t="n">
-        <v>7136</v>
+        <v>5434</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BD-TPF</t>
+          <t>BDS-TPF</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>331</v>
+        <v>175</v>
       </c>
       <c r="C20" t="n">
-        <v>1258</v>
+        <v>696</v>
       </c>
       <c r="D20" t="n">
-        <v>4964</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BD-PPO-TPF</t>
+          <t>BDS-PPO-TPF</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>331</v>
+        <v>175</v>
       </c>
       <c r="C21" t="n">
-        <v>1258</v>
+        <v>696</v>
       </c>
       <c r="D21" t="n">
-        <v>4964</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BD-BRC</t>
+          <t>BDS-BRC</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C22" t="n">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="D22" t="n">
-        <v>404</v>
+        <v>306</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC</t>
+          <t>BDS-PPO-BRC</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C23" t="n">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="D23" t="n">
-        <v>404</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>BD-BRC-TPF</t>
+          <t>BDS-BRC-TPF</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C24" t="n">
-        <v>249</v>
+        <v>165</v>
       </c>
       <c r="D24" t="n">
-        <v>771</v>
+        <v>528</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-TPF</t>
+          <t>BDS-PPO-BRC-TPF</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C25" t="n">
-        <v>249</v>
+        <v>165</v>
       </c>
       <c r="D25" t="n">
-        <v>771</v>
+        <v>528</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BD-GLM</t>
+          <t>BDS-GLM</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>458</v>
+        <v>428</v>
       </c>
       <c r="C26" t="n">
-        <v>1752</v>
+        <v>1473</v>
       </c>
       <c r="D26" t="n">
-        <v>7118</v>
+        <v>6086</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BD-PPO-GLM</t>
+          <t>BDS-PPO-GLM</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>458</v>
+        <v>428</v>
       </c>
       <c r="C27" t="n">
-        <v>1752</v>
+        <v>1473</v>
       </c>
       <c r="D27" t="n">
-        <v>7118</v>
+        <v>6086</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BD-GLM-TPF</t>
+          <t>BDS-GLM-TPF</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>336</v>
+        <v>188</v>
       </c>
       <c r="C28" t="n">
-        <v>1311</v>
+        <v>741</v>
       </c>
       <c r="D28" t="n">
-        <v>5059</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BD-PPO-GLM-TPF</t>
+          <t>BDS-PPO-GLM-TPF</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>336</v>
+        <v>188</v>
       </c>
       <c r="C29" t="n">
-        <v>1311</v>
+        <v>741</v>
       </c>
       <c r="D29" t="n">
-        <v>5059</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BD-BRC-GLM</t>
+          <t>BDS-BRC-GLM</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C30" t="n">
-        <v>213</v>
+        <v>295</v>
       </c>
       <c r="D30" t="n">
-        <v>414</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-GLM</t>
+          <t>BDS-PPO-BRC-GLM</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C31" t="n">
-        <v>213</v>
+        <v>295</v>
       </c>
       <c r="D31" t="n">
-        <v>414</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BD-BRC-GLM-TPF</t>
+          <t>BDS-BRC-GLM-TPF</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C32" t="n">
-        <v>332</v>
+        <v>173</v>
       </c>
       <c r="D32" t="n">
-        <v>1593</v>
+        <v>488</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-GLM-TPF</t>
+          <t>BDS-PPO-BRC-GLM-TPF</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="C33" t="n">
-        <v>332</v>
+        <v>173</v>
       </c>
       <c r="D33" t="n">
-        <v>1593</v>
+        <v>488</v>
       </c>
     </row>
     <row r="34">
@@ -1226,7 +1226,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BD-JPS</t>
+          <t>BDS-JPS</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -1242,7 +1242,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BD-PPO-JPS</t>
+          <t>BDS-PPO-JPS</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -1258,7 +1258,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BD-TPF-JPS</t>
+          <t>BDS-TPF-JPS</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -1274,7 +1274,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BD-PPO-TPF-JPS</t>
+          <t>BDS-PPO-TPF-JPS</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -1290,7 +1290,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BD-BRC-JPS</t>
+          <t>BDS-BRC-JPS</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -1306,7 +1306,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-JPS</t>
+          <t>BDS-PPO-BRC-JPS</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1322,7 +1322,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BD-BRC-TPF-JPS</t>
+          <t>BDS-BRC-TPF-JPS</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1338,7 +1338,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-TPF-JPS</t>
+          <t>BDS-PPO-BRC-TPF-JPS</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1354,7 +1354,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BD-GLM-JPS</t>
+          <t>BDS-GLM-JPS</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -1370,7 +1370,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BD-PPO-GLM-JPS</t>
+          <t>BDS-PPO-GLM-JPS</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1386,7 +1386,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BD-GLM-TPF-JPS</t>
+          <t>BDS-GLM-TPF-JPS</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1402,7 +1402,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BD-PPO-GLM-TPF-JPS</t>
+          <t>BDS-PPO-GLM-TPF-JPS</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1418,7 +1418,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BD-BRC-GLM-JPS</t>
+          <t>BDS-BRC-GLM-JPS</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1434,7 +1434,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-GLM-JPS</t>
+          <t>BDS-PPO-BRC-GLM-JPS</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1450,7 +1450,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BD-BRC-GLM-TPF-JPS</t>
+          <t>BDS-BRC-GLM-TPF-JPS</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1466,7 +1466,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BD-PPO-BRC-GLM-TPF-JPS</t>
+          <t>BDS-PPO-BRC-GLM-TPF-JPS</t>
         </is>
       </c>
       <c r="B65" t="n">

</xml_diff>

<commit_message>
z_pengujian made a proper excel data and indexing to make chart
</commit_message>
<xml_diff>
--- a/Data/Pengujian/closelist_512_Avg10_AllComb.xlsx
+++ b/Data/Pengujian/closelist_512_Avg10_AllComb.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>128</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>256</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>512</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -470,6 +480,12 @@
       <c r="D2" t="n">
         <v>5260</v>
       </c>
+      <c r="E2" t="n">
+        <v>20981</v>
+      </c>
+      <c r="F2" t="n">
+        <v>83814</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -486,6 +502,12 @@
       <c r="D3" t="n">
         <v>5260</v>
       </c>
+      <c r="E3" t="n">
+        <v>20981</v>
+      </c>
+      <c r="F3" t="n">
+        <v>83814</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -502,6 +524,12 @@
       <c r="D4" t="n">
         <v>3648</v>
       </c>
+      <c r="E4" t="n">
+        <v>14364</v>
+      </c>
+      <c r="F4" t="n">
+        <v>57098</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -518,6 +546,12 @@
       <c r="D5" t="n">
         <v>3648</v>
       </c>
+      <c r="E5" t="n">
+        <v>14364</v>
+      </c>
+      <c r="F5" t="n">
+        <v>57098</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -534,6 +568,12 @@
       <c r="D6" t="n">
         <v>590</v>
       </c>
+      <c r="E6" t="n">
+        <v>2798</v>
+      </c>
+      <c r="F6" t="n">
+        <v>13066</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -550,6 +590,12 @@
       <c r="D7" t="n">
         <v>590</v>
       </c>
+      <c r="E7" t="n">
+        <v>2798</v>
+      </c>
+      <c r="F7" t="n">
+        <v>13066</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -566,6 +612,12 @@
       <c r="D8" t="n">
         <v>674</v>
       </c>
+      <c r="E8" t="n">
+        <v>2948</v>
+      </c>
+      <c r="F8" t="n">
+        <v>13197</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -582,6 +634,12 @@
       <c r="D9" t="n">
         <v>674</v>
       </c>
+      <c r="E9" t="n">
+        <v>2948</v>
+      </c>
+      <c r="F9" t="n">
+        <v>13197</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -598,6 +656,12 @@
       <c r="D10" t="n">
         <v>7555</v>
       </c>
+      <c r="E10" t="n">
+        <v>28506</v>
+      </c>
+      <c r="F10" t="n">
+        <v>121920</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -614,6 +678,12 @@
       <c r="D11" t="n">
         <v>7555</v>
       </c>
+      <c r="E11" t="n">
+        <v>28506</v>
+      </c>
+      <c r="F11" t="n">
+        <v>121920</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -630,6 +700,12 @@
       <c r="D12" t="n">
         <v>4095</v>
       </c>
+      <c r="E12" t="n">
+        <v>16743</v>
+      </c>
+      <c r="F12" t="n">
+        <v>67373</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -646,6 +722,12 @@
       <c r="D13" t="n">
         <v>4095</v>
       </c>
+      <c r="E13" t="n">
+        <v>16743</v>
+      </c>
+      <c r="F13" t="n">
+        <v>67373</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -662,6 +744,12 @@
       <c r="D14" t="n">
         <v>614</v>
       </c>
+      <c r="E14" t="n">
+        <v>2813</v>
+      </c>
+      <c r="F14" t="n">
+        <v>13489</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -678,6 +766,12 @@
       <c r="D15" t="n">
         <v>614</v>
       </c>
+      <c r="E15" t="n">
+        <v>2813</v>
+      </c>
+      <c r="F15" t="n">
+        <v>13489</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -694,6 +788,12 @@
       <c r="D16" t="n">
         <v>693</v>
       </c>
+      <c r="E16" t="n">
+        <v>2820</v>
+      </c>
+      <c r="F16" t="n">
+        <v>12398</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -710,6 +810,12 @@
       <c r="D17" t="n">
         <v>693</v>
       </c>
+      <c r="E17" t="n">
+        <v>2820</v>
+      </c>
+      <c r="F17" t="n">
+        <v>12398</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -726,6 +832,12 @@
       <c r="D18" t="n">
         <v>5434</v>
       </c>
+      <c r="E18" t="n">
+        <v>21165</v>
+      </c>
+      <c r="F18" t="n">
+        <v>83808</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -742,6 +854,12 @@
       <c r="D19" t="n">
         <v>5434</v>
       </c>
+      <c r="E19" t="n">
+        <v>21165</v>
+      </c>
+      <c r="F19" t="n">
+        <v>83808</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -758,6 +876,12 @@
       <c r="D20" t="n">
         <v>2697</v>
       </c>
+      <c r="E20" t="n">
+        <v>10442</v>
+      </c>
+      <c r="F20" t="n">
+        <v>41349</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -774,6 +898,12 @@
       <c r="D21" t="n">
         <v>2697</v>
       </c>
+      <c r="E21" t="n">
+        <v>10442</v>
+      </c>
+      <c r="F21" t="n">
+        <v>41349</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -790,6 +920,12 @@
       <c r="D22" t="n">
         <v>306</v>
       </c>
+      <c r="E22" t="n">
+        <v>3595</v>
+      </c>
+      <c r="F22" t="n">
+        <v>14442</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -806,6 +942,12 @@
       <c r="D23" t="n">
         <v>306</v>
       </c>
+      <c r="E23" t="n">
+        <v>3595</v>
+      </c>
+      <c r="F23" t="n">
+        <v>14442</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -822,6 +964,12 @@
       <c r="D24" t="n">
         <v>528</v>
       </c>
+      <c r="E24" t="n">
+        <v>1651</v>
+      </c>
+      <c r="F24" t="n">
+        <v>5672</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -838,6 +986,12 @@
       <c r="D25" t="n">
         <v>528</v>
       </c>
+      <c r="E25" t="n">
+        <v>1651</v>
+      </c>
+      <c r="F25" t="n">
+        <v>5672</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -854,6 +1008,12 @@
       <c r="D26" t="n">
         <v>6086</v>
       </c>
+      <c r="E26" t="n">
+        <v>23293</v>
+      </c>
+      <c r="F26" t="n">
+        <v>95312</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -870,6 +1030,12 @@
       <c r="D27" t="n">
         <v>6086</v>
       </c>
+      <c r="E27" t="n">
+        <v>23293</v>
+      </c>
+      <c r="F27" t="n">
+        <v>95312</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -886,6 +1052,12 @@
       <c r="D28" t="n">
         <v>2672</v>
       </c>
+      <c r="E28" t="n">
+        <v>10273</v>
+      </c>
+      <c r="F28" t="n">
+        <v>41118</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -902,6 +1074,12 @@
       <c r="D29" t="n">
         <v>2672</v>
       </c>
+      <c r="E29" t="n">
+        <v>10273</v>
+      </c>
+      <c r="F29" t="n">
+        <v>41118</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -918,6 +1096,12 @@
       <c r="D30" t="n">
         <v>1087</v>
       </c>
+      <c r="E30" t="n">
+        <v>5449</v>
+      </c>
+      <c r="F30" t="n">
+        <v>22623</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -934,6 +1118,12 @@
       <c r="D31" t="n">
         <v>1087</v>
       </c>
+      <c r="E31" t="n">
+        <v>5449</v>
+      </c>
+      <c r="F31" t="n">
+        <v>22623</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -950,6 +1140,12 @@
       <c r="D32" t="n">
         <v>488</v>
       </c>
+      <c r="E32" t="n">
+        <v>673</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2001</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -966,6 +1162,12 @@
       <c r="D33" t="n">
         <v>488</v>
       </c>
+      <c r="E33" t="n">
+        <v>673</v>
+      </c>
+      <c r="F33" t="n">
+        <v>2001</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -982,6 +1184,12 @@
       <c r="D34" t="n">
         <v>87</v>
       </c>
+      <c r="E34" t="n">
+        <v>87</v>
+      </c>
+      <c r="F34" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -998,6 +1206,12 @@
       <c r="D35" t="n">
         <v>87</v>
       </c>
+      <c r="E35" t="n">
+        <v>87</v>
+      </c>
+      <c r="F35" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1014,6 +1228,12 @@
       <c r="D36" t="n">
         <v>74</v>
       </c>
+      <c r="E36" t="n">
+        <v>74</v>
+      </c>
+      <c r="F36" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1030,6 +1250,12 @@
       <c r="D37" t="n">
         <v>74</v>
       </c>
+      <c r="E37" t="n">
+        <v>74</v>
+      </c>
+      <c r="F37" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1046,6 +1272,12 @@
       <c r="D38" t="n">
         <v>30</v>
       </c>
+      <c r="E38" t="n">
+        <v>30</v>
+      </c>
+      <c r="F38" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1062,6 +1294,12 @@
       <c r="D39" t="n">
         <v>30</v>
       </c>
+      <c r="E39" t="n">
+        <v>30</v>
+      </c>
+      <c r="F39" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1078,6 +1316,12 @@
       <c r="D40" t="n">
         <v>30</v>
       </c>
+      <c r="E40" t="n">
+        <v>30</v>
+      </c>
+      <c r="F40" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1094,6 +1338,12 @@
       <c r="D41" t="n">
         <v>30</v>
       </c>
+      <c r="E41" t="n">
+        <v>30</v>
+      </c>
+      <c r="F41" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1110,6 +1360,12 @@
       <c r="D42" t="n">
         <v>131</v>
       </c>
+      <c r="E42" t="n">
+        <v>158</v>
+      </c>
+      <c r="F42" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1126,6 +1382,12 @@
       <c r="D43" t="n">
         <v>131</v>
       </c>
+      <c r="E43" t="n">
+        <v>158</v>
+      </c>
+      <c r="F43" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1142,6 +1404,12 @@
       <c r="D44" t="n">
         <v>140</v>
       </c>
+      <c r="E44" t="n">
+        <v>149</v>
+      </c>
+      <c r="F44" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1158,6 +1426,12 @@
       <c r="D45" t="n">
         <v>140</v>
       </c>
+      <c r="E45" t="n">
+        <v>149</v>
+      </c>
+      <c r="F45" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1174,6 +1448,12 @@
       <c r="D46" t="n">
         <v>106</v>
       </c>
+      <c r="E46" t="n">
+        <v>149</v>
+      </c>
+      <c r="F46" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1190,6 +1470,12 @@
       <c r="D47" t="n">
         <v>106</v>
       </c>
+      <c r="E47" t="n">
+        <v>149</v>
+      </c>
+      <c r="F47" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1206,6 +1492,12 @@
       <c r="D48" t="n">
         <v>104</v>
       </c>
+      <c r="E48" t="n">
+        <v>116</v>
+      </c>
+      <c r="F48" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1222,6 +1514,12 @@
       <c r="D49" t="n">
         <v>104</v>
       </c>
+      <c r="E49" t="n">
+        <v>116</v>
+      </c>
+      <c r="F49" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1238,6 +1536,12 @@
       <c r="D50" t="n">
         <v>29</v>
       </c>
+      <c r="E50" t="n">
+        <v>29</v>
+      </c>
+      <c r="F50" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1254,6 +1558,12 @@
       <c r="D51" t="n">
         <v>29</v>
       </c>
+      <c r="E51" t="n">
+        <v>29</v>
+      </c>
+      <c r="F51" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1270,6 +1580,12 @@
       <c r="D52" t="n">
         <v>40</v>
       </c>
+      <c r="E52" t="n">
+        <v>40</v>
+      </c>
+      <c r="F52" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1286,6 +1602,12 @@
       <c r="D53" t="n">
         <v>40</v>
       </c>
+      <c r="E53" t="n">
+        <v>40</v>
+      </c>
+      <c r="F53" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1302,6 +1624,12 @@
       <c r="D54" t="n">
         <v>33</v>
       </c>
+      <c r="E54" t="n">
+        <v>33</v>
+      </c>
+      <c r="F54" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1318,6 +1646,12 @@
       <c r="D55" t="n">
         <v>33</v>
       </c>
+      <c r="E55" t="n">
+        <v>33</v>
+      </c>
+      <c r="F55" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1334,6 +1668,12 @@
       <c r="D56" t="n">
         <v>36</v>
       </c>
+      <c r="E56" t="n">
+        <v>36</v>
+      </c>
+      <c r="F56" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1350,6 +1690,12 @@
       <c r="D57" t="n">
         <v>36</v>
       </c>
+      <c r="E57" t="n">
+        <v>36</v>
+      </c>
+      <c r="F57" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1366,6 +1712,12 @@
       <c r="D58" t="n">
         <v>62</v>
       </c>
+      <c r="E58" t="n">
+        <v>94</v>
+      </c>
+      <c r="F58" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1382,6 +1734,12 @@
       <c r="D59" t="n">
         <v>62</v>
       </c>
+      <c r="E59" t="n">
+        <v>94</v>
+      </c>
+      <c r="F59" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1398,6 +1756,12 @@
       <c r="D60" t="n">
         <v>68</v>
       </c>
+      <c r="E60" t="n">
+        <v>95</v>
+      </c>
+      <c r="F60" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1414,6 +1778,12 @@
       <c r="D61" t="n">
         <v>68</v>
       </c>
+      <c r="E61" t="n">
+        <v>95</v>
+      </c>
+      <c r="F61" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1430,6 +1800,12 @@
       <c r="D62" t="n">
         <v>64</v>
       </c>
+      <c r="E62" t="n">
+        <v>80</v>
+      </c>
+      <c r="F62" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1446,6 +1822,12 @@
       <c r="D63" t="n">
         <v>64</v>
       </c>
+      <c r="E63" t="n">
+        <v>80</v>
+      </c>
+      <c r="F63" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1462,6 +1844,12 @@
       <c r="D64" t="n">
         <v>68</v>
       </c>
+      <c r="E64" t="n">
+        <v>80</v>
+      </c>
+      <c r="F64" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1477,6 +1865,12 @@
       </c>
       <c r="D65" t="n">
         <v>68</v>
+      </c>
+      <c r="E65" t="n">
+        <v>80</v>
+      </c>
+      <c r="F65" t="n">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>